<commit_message>
adding executive summary, comparison with competitors, smarteye
</commit_message>
<xml_diff>
--- a/AR VR Company/Top AR VR Company Financials.xlsx
+++ b/AR VR Company/Top AR VR Company Financials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nugroho/Dropbox/AR VR Analysis/AR VR Company/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E0EAAB-D502-284E-B7CB-8336C6E39418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C32B62A-83D0-2C4C-A14F-9EE8F3F10A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="1480" windowWidth="21860" windowHeight="13020" activeTab="2" xr2:uid="{37DBE269-0922-714C-BDB9-DADB377AD4AA}"/>
+    <workbookView xWindow="1080" yWindow="640" windowWidth="21860" windowHeight="13020" xr2:uid="{37DBE269-0922-714C-BDB9-DADB377AD4AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="FB" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -795,7 +796,18 @@
     <xf numFmtId="9" fontId="0" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -803,6 +815,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -827,20 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1162,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70158042-C05D-2046-A88C-F64D24D92654}">
   <dimension ref="A1:FF10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1206,403 +1207,403 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:162">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="67" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="62" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62" t="s">
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62" t="s">
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="62" t="s">
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67"/>
+      <c r="AK1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="62" t="s">
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="62"/>
-      <c r="AV1" s="62"/>
-      <c r="AW1" s="62"/>
-      <c r="AX1" s="62"/>
-      <c r="AY1" s="62" t="s">
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="67"/>
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67"/>
+      <c r="AY1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AZ1" s="62"/>
-      <c r="BA1" s="62"/>
-      <c r="BB1" s="62"/>
-      <c r="BC1" s="62"/>
-      <c r="BD1" s="62"/>
-      <c r="BE1" s="62"/>
-      <c r="BF1" s="62" t="s">
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="BG1" s="62"/>
-      <c r="BH1" s="62"/>
-      <c r="BI1" s="62"/>
-      <c r="BJ1" s="62"/>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="62"/>
-      <c r="BM1" s="63" t="s">
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="63"/>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="63"/>
-      <c r="BT1" s="63" t="s">
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="68"/>
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68"/>
+      <c r="BT1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="63"/>
-      <c r="BX1" s="63"/>
-      <c r="BY1" s="63"/>
-      <c r="BZ1" s="63"/>
-      <c r="CA1" s="63" t="s">
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="68"/>
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68"/>
+      <c r="CA1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="CB1" s="63"/>
-      <c r="CC1" s="63"/>
-      <c r="CD1" s="63"/>
-      <c r="CE1" s="63"/>
-      <c r="CF1" s="63"/>
-      <c r="CG1" s="63"/>
-      <c r="CH1" s="62" t="s">
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="68"/>
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="68"/>
+      <c r="CH1" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="CI1" s="62"/>
-      <c r="CJ1" s="62"/>
-      <c r="CK1" s="62"/>
-      <c r="CL1" s="62"/>
-      <c r="CM1" s="62"/>
-      <c r="CN1" s="62"/>
-      <c r="CO1" s="62" t="s">
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="CP1" s="62"/>
-      <c r="CQ1" s="62"/>
-      <c r="CR1" s="62"/>
-      <c r="CS1" s="62"/>
-      <c r="CT1" s="62"/>
-      <c r="CU1" s="62"/>
-      <c r="CV1" s="62" t="s">
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67"/>
+      <c r="CV1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="CW1" s="62"/>
-      <c r="CX1" s="62"/>
-      <c r="CY1" s="62"/>
-      <c r="CZ1" s="62"/>
-      <c r="DA1" s="62"/>
-      <c r="DB1" s="62"/>
-      <c r="DC1" s="62" t="s">
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="67"/>
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67"/>
+      <c r="DC1" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="DD1" s="62"/>
-      <c r="DE1" s="62"/>
-      <c r="DF1" s="62"/>
-      <c r="DG1" s="62"/>
-      <c r="DH1" s="62"/>
-      <c r="DI1" s="62"/>
-      <c r="DJ1" s="62" t="s">
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
+      <c r="DF1" s="67"/>
+      <c r="DG1" s="67"/>
+      <c r="DH1" s="67"/>
+      <c r="DI1" s="67"/>
+      <c r="DJ1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="DK1" s="62"/>
-      <c r="DL1" s="62"/>
-      <c r="DM1" s="62"/>
-      <c r="DN1" s="62"/>
-      <c r="DO1" s="62"/>
-      <c r="DP1" s="62"/>
-      <c r="DQ1" s="62" t="s">
+      <c r="DK1" s="67"/>
+      <c r="DL1" s="67"/>
+      <c r="DM1" s="67"/>
+      <c r="DN1" s="67"/>
+      <c r="DO1" s="67"/>
+      <c r="DP1" s="67"/>
+      <c r="DQ1" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="DR1" s="62"/>
-      <c r="DS1" s="62"/>
-      <c r="DT1" s="62"/>
-      <c r="DU1" s="62"/>
-      <c r="DV1" s="62"/>
-      <c r="DW1" s="62"/>
-      <c r="DX1" s="62" t="s">
+      <c r="DR1" s="67"/>
+      <c r="DS1" s="67"/>
+      <c r="DT1" s="67"/>
+      <c r="DU1" s="67"/>
+      <c r="DV1" s="67"/>
+      <c r="DW1" s="67"/>
+      <c r="DX1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="DY1" s="62"/>
-      <c r="DZ1" s="62"/>
-      <c r="EA1" s="62"/>
-      <c r="EB1" s="62"/>
-      <c r="EC1" s="62"/>
-      <c r="ED1" s="62"/>
-      <c r="EE1" s="62" t="s">
+      <c r="DY1" s="67"/>
+      <c r="DZ1" s="67"/>
+      <c r="EA1" s="67"/>
+      <c r="EB1" s="67"/>
+      <c r="EC1" s="67"/>
+      <c r="ED1" s="67"/>
+      <c r="EE1" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="EF1" s="62"/>
-      <c r="EG1" s="62"/>
-      <c r="EH1" s="62"/>
-      <c r="EI1" s="62"/>
-      <c r="EJ1" s="62"/>
-      <c r="EK1" s="62"/>
-      <c r="EL1" s="61" t="s">
+      <c r="EF1" s="67"/>
+      <c r="EG1" s="67"/>
+      <c r="EH1" s="67"/>
+      <c r="EI1" s="67"/>
+      <c r="EJ1" s="67"/>
+      <c r="EK1" s="67"/>
+      <c r="EL1" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="EM1" s="61"/>
-      <c r="EN1" s="61"/>
-      <c r="EO1" s="61"/>
-      <c r="EP1" s="61"/>
-      <c r="EQ1" s="61"/>
-      <c r="ER1" s="61"/>
-      <c r="ES1" s="61" t="s">
+      <c r="EM1" s="69"/>
+      <c r="EN1" s="69"/>
+      <c r="EO1" s="69"/>
+      <c r="EP1" s="69"/>
+      <c r="EQ1" s="69"/>
+      <c r="ER1" s="69"/>
+      <c r="ES1" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="ET1" s="61"/>
-      <c r="EU1" s="61"/>
-      <c r="EV1" s="61"/>
-      <c r="EW1" s="61"/>
-      <c r="EX1" s="61"/>
-      <c r="EY1" s="61"/>
-      <c r="EZ1" s="61" t="s">
+      <c r="ET1" s="69"/>
+      <c r="EU1" s="69"/>
+      <c r="EV1" s="69"/>
+      <c r="EW1" s="69"/>
+      <c r="EX1" s="69"/>
+      <c r="EY1" s="69"/>
+      <c r="EZ1" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="FA1" s="61"/>
-      <c r="FB1" s="61"/>
-      <c r="FC1" s="61"/>
-      <c r="FD1" s="61"/>
-      <c r="FE1" s="61"/>
-      <c r="FF1" s="61"/>
+      <c r="FA1" s="69"/>
+      <c r="FB1" s="69"/>
+      <c r="FC1" s="69"/>
+      <c r="FD1" s="69"/>
+      <c r="FE1" s="69"/>
+      <c r="FF1" s="69"/>
     </row>
     <row r="2" spans="1:162">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="62"/>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="62"/>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="62"/>
-      <c r="AV2" s="62"/>
-      <c r="AW2" s="62"/>
-      <c r="AX2" s="62"/>
-      <c r="AY2" s="62"/>
-      <c r="AZ2" s="62"/>
-      <c r="BA2" s="62"/>
-      <c r="BB2" s="62"/>
-      <c r="BC2" s="62"/>
-      <c r="BD2" s="62"/>
-      <c r="BE2" s="62"/>
-      <c r="BF2" s="62"/>
-      <c r="BG2" s="62"/>
-      <c r="BH2" s="62"/>
-      <c r="BI2" s="62"/>
-      <c r="BJ2" s="62"/>
-      <c r="BK2" s="62"/>
-      <c r="BL2" s="62"/>
-      <c r="BM2" s="63"/>
-      <c r="BN2" s="63"/>
-      <c r="BO2" s="63"/>
-      <c r="BP2" s="63"/>
-      <c r="BQ2" s="63"/>
-      <c r="BR2" s="63"/>
-      <c r="BS2" s="63"/>
-      <c r="BT2" s="63"/>
-      <c r="BU2" s="63"/>
-      <c r="BV2" s="63"/>
-      <c r="BW2" s="63"/>
-      <c r="BX2" s="63"/>
-      <c r="BY2" s="63"/>
-      <c r="BZ2" s="63"/>
-      <c r="CA2" s="63"/>
-      <c r="CB2" s="63"/>
-      <c r="CC2" s="63"/>
-      <c r="CD2" s="63"/>
-      <c r="CE2" s="63"/>
-      <c r="CF2" s="63"/>
-      <c r="CG2" s="63"/>
-      <c r="CH2" s="62" t="s">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67"/>
+      <c r="AJ2" s="67"/>
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="67"/>
+      <c r="AM2" s="67"/>
+      <c r="AN2" s="67"/>
+      <c r="AO2" s="67"/>
+      <c r="AP2" s="67"/>
+      <c r="AQ2" s="67"/>
+      <c r="AR2" s="67"/>
+      <c r="AS2" s="67"/>
+      <c r="AT2" s="67"/>
+      <c r="AU2" s="67"/>
+      <c r="AV2" s="67"/>
+      <c r="AW2" s="67"/>
+      <c r="AX2" s="67"/>
+      <c r="AY2" s="67"/>
+      <c r="AZ2" s="67"/>
+      <c r="BA2" s="67"/>
+      <c r="BB2" s="67"/>
+      <c r="BC2" s="67"/>
+      <c r="BD2" s="67"/>
+      <c r="BE2" s="67"/>
+      <c r="BF2" s="67"/>
+      <c r="BG2" s="67"/>
+      <c r="BH2" s="67"/>
+      <c r="BI2" s="67"/>
+      <c r="BJ2" s="67"/>
+      <c r="BK2" s="67"/>
+      <c r="BL2" s="67"/>
+      <c r="BM2" s="68"/>
+      <c r="BN2" s="68"/>
+      <c r="BO2" s="68"/>
+      <c r="BP2" s="68"/>
+      <c r="BQ2" s="68"/>
+      <c r="BR2" s="68"/>
+      <c r="BS2" s="68"/>
+      <c r="BT2" s="68"/>
+      <c r="BU2" s="68"/>
+      <c r="BV2" s="68"/>
+      <c r="BW2" s="68"/>
+      <c r="BX2" s="68"/>
+      <c r="BY2" s="68"/>
+      <c r="BZ2" s="68"/>
+      <c r="CA2" s="68"/>
+      <c r="CB2" s="68"/>
+      <c r="CC2" s="68"/>
+      <c r="CD2" s="68"/>
+      <c r="CE2" s="68"/>
+      <c r="CF2" s="68"/>
+      <c r="CG2" s="68"/>
+      <c r="CH2" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="CI2" s="62"/>
-      <c r="CJ2" s="62"/>
-      <c r="CK2" s="62"/>
-      <c r="CL2" s="62"/>
-      <c r="CM2" s="62"/>
-      <c r="CN2" s="62"/>
-      <c r="CO2" s="62" t="s">
+      <c r="CI2" s="67"/>
+      <c r="CJ2" s="67"/>
+      <c r="CK2" s="67"/>
+      <c r="CL2" s="67"/>
+      <c r="CM2" s="67"/>
+      <c r="CN2" s="67"/>
+      <c r="CO2" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="CP2" s="62"/>
-      <c r="CQ2" s="62"/>
-      <c r="CR2" s="62"/>
-      <c r="CS2" s="62"/>
-      <c r="CT2" s="62"/>
-      <c r="CU2" s="62"/>
-      <c r="CV2" s="62" t="s">
+      <c r="CP2" s="67"/>
+      <c r="CQ2" s="67"/>
+      <c r="CR2" s="67"/>
+      <c r="CS2" s="67"/>
+      <c r="CT2" s="67"/>
+      <c r="CU2" s="67"/>
+      <c r="CV2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="CW2" s="62"/>
-      <c r="CX2" s="62"/>
-      <c r="CY2" s="62"/>
-      <c r="CZ2" s="62"/>
-      <c r="DA2" s="62"/>
-      <c r="DB2" s="62"/>
-      <c r="DC2" s="62" t="s">
+      <c r="CW2" s="67"/>
+      <c r="CX2" s="67"/>
+      <c r="CY2" s="67"/>
+      <c r="CZ2" s="67"/>
+      <c r="DA2" s="67"/>
+      <c r="DB2" s="67"/>
+      <c r="DC2" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="DD2" s="62"/>
-      <c r="DE2" s="62"/>
-      <c r="DF2" s="62"/>
-      <c r="DG2" s="62"/>
-      <c r="DH2" s="62"/>
-      <c r="DI2" s="62"/>
-      <c r="DJ2" s="62" t="s">
+      <c r="DD2" s="67"/>
+      <c r="DE2" s="67"/>
+      <c r="DF2" s="67"/>
+      <c r="DG2" s="67"/>
+      <c r="DH2" s="67"/>
+      <c r="DI2" s="67"/>
+      <c r="DJ2" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="DK2" s="62"/>
-      <c r="DL2" s="62"/>
-      <c r="DM2" s="62"/>
-      <c r="DN2" s="62"/>
-      <c r="DO2" s="62"/>
-      <c r="DP2" s="62"/>
-      <c r="DQ2" s="62" t="s">
+      <c r="DK2" s="67"/>
+      <c r="DL2" s="67"/>
+      <c r="DM2" s="67"/>
+      <c r="DN2" s="67"/>
+      <c r="DO2" s="67"/>
+      <c r="DP2" s="67"/>
+      <c r="DQ2" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="DR2" s="62"/>
-      <c r="DS2" s="62"/>
-      <c r="DT2" s="62"/>
-      <c r="DU2" s="62"/>
-      <c r="DV2" s="62"/>
-      <c r="DW2" s="62"/>
-      <c r="DX2" s="62" t="s">
+      <c r="DR2" s="67"/>
+      <c r="DS2" s="67"/>
+      <c r="DT2" s="67"/>
+      <c r="DU2" s="67"/>
+      <c r="DV2" s="67"/>
+      <c r="DW2" s="67"/>
+      <c r="DX2" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="DY2" s="62"/>
-      <c r="DZ2" s="62"/>
-      <c r="EA2" s="62"/>
-      <c r="EB2" s="62"/>
-      <c r="EC2" s="62"/>
-      <c r="ED2" s="62"/>
-      <c r="EE2" s="62"/>
-      <c r="EF2" s="62"/>
-      <c r="EG2" s="62"/>
-      <c r="EH2" s="62"/>
-      <c r="EI2" s="62"/>
-      <c r="EJ2" s="62"/>
-      <c r="EK2" s="62"/>
-      <c r="EL2" s="61" t="s">
+      <c r="DY2" s="67"/>
+      <c r="DZ2" s="67"/>
+      <c r="EA2" s="67"/>
+      <c r="EB2" s="67"/>
+      <c r="EC2" s="67"/>
+      <c r="ED2" s="67"/>
+      <c r="EE2" s="67"/>
+      <c r="EF2" s="67"/>
+      <c r="EG2" s="67"/>
+      <c r="EH2" s="67"/>
+      <c r="EI2" s="67"/>
+      <c r="EJ2" s="67"/>
+      <c r="EK2" s="67"/>
+      <c r="EL2" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="EM2" s="61"/>
-      <c r="EN2" s="61"/>
-      <c r="EO2" s="61"/>
-      <c r="EP2" s="61"/>
-      <c r="EQ2" s="61"/>
-      <c r="ER2" s="61"/>
-      <c r="ES2" s="61" t="s">
+      <c r="EM2" s="69"/>
+      <c r="EN2" s="69"/>
+      <c r="EO2" s="69"/>
+      <c r="EP2" s="69"/>
+      <c r="EQ2" s="69"/>
+      <c r="ER2" s="69"/>
+      <c r="ES2" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="ET2" s="61"/>
-      <c r="EU2" s="61"/>
-      <c r="EV2" s="61"/>
-      <c r="EW2" s="61"/>
-      <c r="EX2" s="61"/>
-      <c r="EY2" s="61"/>
-      <c r="EZ2" s="61" t="s">
+      <c r="ET2" s="69"/>
+      <c r="EU2" s="69"/>
+      <c r="EV2" s="69"/>
+      <c r="EW2" s="69"/>
+      <c r="EX2" s="69"/>
+      <c r="EY2" s="69"/>
+      <c r="EZ2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="FA2" s="61"/>
-      <c r="FB2" s="61"/>
-      <c r="FC2" s="61"/>
-      <c r="FD2" s="61"/>
-      <c r="FE2" s="61"/>
-      <c r="FF2" s="61"/>
+      <c r="FA2" s="69"/>
+      <c r="FB2" s="69"/>
+      <c r="FC2" s="69"/>
+      <c r="FD2" s="69"/>
+      <c r="FE2" s="69"/>
+      <c r="FF2" s="69"/>
     </row>
     <row r="3" spans="1:162">
       <c r="E3" s="1">
@@ -2348,6 +2349,10 @@
       <c r="O8" s="3">
         <v>23740</v>
       </c>
+      <c r="P8">
+        <f>(2443+2121+2343)/3*4</f>
+        <v>9209.3333333333339</v>
+      </c>
       <c r="R8" s="7"/>
     </row>
     <row r="9" spans="1:162">
@@ -2428,6 +2433,26 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="ES1:EY1"/>
+    <mergeCell ref="ES2:EY2"/>
+    <mergeCell ref="EZ1:FF1"/>
+    <mergeCell ref="EZ2:FF2"/>
+    <mergeCell ref="DX1:ED1"/>
+    <mergeCell ref="DX2:ED2"/>
+    <mergeCell ref="EE1:EK1"/>
+    <mergeCell ref="EE2:EK2"/>
+    <mergeCell ref="EL1:ER1"/>
+    <mergeCell ref="EL2:ER2"/>
+    <mergeCell ref="CO2:CU2"/>
+    <mergeCell ref="CH1:CN1"/>
+    <mergeCell ref="DQ1:DW1"/>
+    <mergeCell ref="DQ2:DW2"/>
+    <mergeCell ref="K1:S2"/>
+    <mergeCell ref="AK1:AQ2"/>
+    <mergeCell ref="AC1:AJ2"/>
+    <mergeCell ref="DJ1:DP1"/>
+    <mergeCell ref="DJ2:DP2"/>
+    <mergeCell ref="CO1:CU1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:C2"/>
@@ -2444,26 +2469,6 @@
     <mergeCell ref="CH2:CN2"/>
     <mergeCell ref="CV1:DB1"/>
     <mergeCell ref="CV2:DB2"/>
-    <mergeCell ref="CO2:CU2"/>
-    <mergeCell ref="CH1:CN1"/>
-    <mergeCell ref="DQ1:DW1"/>
-    <mergeCell ref="DQ2:DW2"/>
-    <mergeCell ref="K1:S2"/>
-    <mergeCell ref="AK1:AQ2"/>
-    <mergeCell ref="AC1:AJ2"/>
-    <mergeCell ref="DJ1:DP1"/>
-    <mergeCell ref="DJ2:DP2"/>
-    <mergeCell ref="CO1:CU1"/>
-    <mergeCell ref="ES1:EY1"/>
-    <mergeCell ref="ES2:EY2"/>
-    <mergeCell ref="EZ1:FF1"/>
-    <mergeCell ref="EZ2:FF2"/>
-    <mergeCell ref="DX1:ED1"/>
-    <mergeCell ref="DX2:ED2"/>
-    <mergeCell ref="EE1:EK1"/>
-    <mergeCell ref="EE2:EK2"/>
-    <mergeCell ref="EL1:ER1"/>
-    <mergeCell ref="EL2:ER2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2515,401 +2520,401 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:161">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="67" t="s">
         <v>35</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="62" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62" t="s">
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62" t="s">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62" t="s">
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62" t="s">
+      <c r="AK1" s="67"/>
+      <c r="AL1" s="67"/>
+      <c r="AM1" s="67"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="62"/>
-      <c r="AV1" s="62"/>
-      <c r="AW1" s="62"/>
-      <c r="AX1" s="62" t="s">
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="67"/>
+      <c r="AT1" s="67"/>
+      <c r="AU1" s="67"/>
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="67"/>
+      <c r="AX1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="AY1" s="62"/>
-      <c r="AZ1" s="62"/>
-      <c r="BA1" s="62"/>
-      <c r="BB1" s="62"/>
-      <c r="BC1" s="62"/>
-      <c r="BD1" s="62"/>
-      <c r="BE1" s="62" t="s">
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="BF1" s="62"/>
-      <c r="BG1" s="62"/>
-      <c r="BH1" s="62"/>
-      <c r="BI1" s="62"/>
-      <c r="BJ1" s="62"/>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="63" t="s">
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="BM1" s="63"/>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="63"/>
-      <c r="BP1" s="63"/>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="63" t="s">
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="68"/>
+      <c r="BP1" s="68"/>
+      <c r="BQ1" s="68"/>
+      <c r="BR1" s="68"/>
+      <c r="BS1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="63"/>
-      <c r="BX1" s="63"/>
-      <c r="BY1" s="63"/>
-      <c r="BZ1" s="63" t="s">
+      <c r="BT1" s="68"/>
+      <c r="BU1" s="68"/>
+      <c r="BV1" s="68"/>
+      <c r="BW1" s="68"/>
+      <c r="BX1" s="68"/>
+      <c r="BY1" s="68"/>
+      <c r="BZ1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="CA1" s="63"/>
-      <c r="CB1" s="63"/>
-      <c r="CC1" s="63"/>
-      <c r="CD1" s="63"/>
-      <c r="CE1" s="63"/>
-      <c r="CF1" s="63"/>
-      <c r="CG1" s="62" t="s">
+      <c r="CA1" s="68"/>
+      <c r="CB1" s="68"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="68"/>
+      <c r="CE1" s="68"/>
+      <c r="CF1" s="68"/>
+      <c r="CG1" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="CH1" s="62"/>
-      <c r="CI1" s="62"/>
-      <c r="CJ1" s="62"/>
-      <c r="CK1" s="62"/>
-      <c r="CL1" s="62"/>
-      <c r="CM1" s="62"/>
-      <c r="CN1" s="62" t="s">
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="CO1" s="62"/>
-      <c r="CP1" s="62"/>
-      <c r="CQ1" s="62"/>
-      <c r="CR1" s="62"/>
-      <c r="CS1" s="62"/>
-      <c r="CT1" s="62"/>
-      <c r="CU1" s="62" t="s">
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="67"/>
+      <c r="CT1" s="67"/>
+      <c r="CU1" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="CV1" s="62"/>
-      <c r="CW1" s="62"/>
-      <c r="CX1" s="62"/>
-      <c r="CY1" s="62"/>
-      <c r="CZ1" s="62"/>
-      <c r="DA1" s="62"/>
-      <c r="DB1" s="62" t="s">
+      <c r="CV1" s="67"/>
+      <c r="CW1" s="67"/>
+      <c r="CX1" s="67"/>
+      <c r="CY1" s="67"/>
+      <c r="CZ1" s="67"/>
+      <c r="DA1" s="67"/>
+      <c r="DB1" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="DC1" s="62"/>
-      <c r="DD1" s="62"/>
-      <c r="DE1" s="62"/>
-      <c r="DF1" s="62"/>
-      <c r="DG1" s="62"/>
-      <c r="DH1" s="62"/>
-      <c r="DI1" s="62" t="s">
+      <c r="DC1" s="67"/>
+      <c r="DD1" s="67"/>
+      <c r="DE1" s="67"/>
+      <c r="DF1" s="67"/>
+      <c r="DG1" s="67"/>
+      <c r="DH1" s="67"/>
+      <c r="DI1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="DJ1" s="62"/>
-      <c r="DK1" s="62"/>
-      <c r="DL1" s="62"/>
-      <c r="DM1" s="62"/>
-      <c r="DN1" s="62"/>
-      <c r="DO1" s="62"/>
-      <c r="DP1" s="62" t="s">
+      <c r="DJ1" s="67"/>
+      <c r="DK1" s="67"/>
+      <c r="DL1" s="67"/>
+      <c r="DM1" s="67"/>
+      <c r="DN1" s="67"/>
+      <c r="DO1" s="67"/>
+      <c r="DP1" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="DQ1" s="62"/>
-      <c r="DR1" s="62"/>
-      <c r="DS1" s="62"/>
-      <c r="DT1" s="62"/>
-      <c r="DU1" s="62"/>
-      <c r="DV1" s="62"/>
-      <c r="DW1" s="62" t="s">
+      <c r="DQ1" s="67"/>
+      <c r="DR1" s="67"/>
+      <c r="DS1" s="67"/>
+      <c r="DT1" s="67"/>
+      <c r="DU1" s="67"/>
+      <c r="DV1" s="67"/>
+      <c r="DW1" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="DX1" s="62"/>
-      <c r="DY1" s="62"/>
-      <c r="DZ1" s="62"/>
-      <c r="EA1" s="62"/>
-      <c r="EB1" s="62"/>
-      <c r="EC1" s="62"/>
-      <c r="ED1" s="62" t="s">
+      <c r="DX1" s="67"/>
+      <c r="DY1" s="67"/>
+      <c r="DZ1" s="67"/>
+      <c r="EA1" s="67"/>
+      <c r="EB1" s="67"/>
+      <c r="EC1" s="67"/>
+      <c r="ED1" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="EE1" s="62"/>
-      <c r="EF1" s="62"/>
-      <c r="EG1" s="62"/>
-      <c r="EH1" s="62"/>
-      <c r="EI1" s="62"/>
-      <c r="EJ1" s="62"/>
-      <c r="EK1" s="61" t="s">
+      <c r="EE1" s="67"/>
+      <c r="EF1" s="67"/>
+      <c r="EG1" s="67"/>
+      <c r="EH1" s="67"/>
+      <c r="EI1" s="67"/>
+      <c r="EJ1" s="67"/>
+      <c r="EK1" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="EL1" s="61"/>
-      <c r="EM1" s="61"/>
-      <c r="EN1" s="61"/>
-      <c r="EO1" s="61"/>
-      <c r="EP1" s="61"/>
-      <c r="EQ1" s="61"/>
-      <c r="ER1" s="61" t="s">
+      <c r="EL1" s="69"/>
+      <c r="EM1" s="69"/>
+      <c r="EN1" s="69"/>
+      <c r="EO1" s="69"/>
+      <c r="EP1" s="69"/>
+      <c r="EQ1" s="69"/>
+      <c r="ER1" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="ES1" s="61"/>
-      <c r="ET1" s="61"/>
-      <c r="EU1" s="61"/>
-      <c r="EV1" s="61"/>
-      <c r="EW1" s="61"/>
-      <c r="EX1" s="61"/>
-      <c r="EY1" s="61" t="s">
+      <c r="ES1" s="69"/>
+      <c r="ET1" s="69"/>
+      <c r="EU1" s="69"/>
+      <c r="EV1" s="69"/>
+      <c r="EW1" s="69"/>
+      <c r="EX1" s="69"/>
+      <c r="EY1" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="EZ1" s="61"/>
-      <c r="FA1" s="61"/>
-      <c r="FB1" s="61"/>
-      <c r="FC1" s="61"/>
-      <c r="FD1" s="61"/>
-      <c r="FE1" s="61"/>
+      <c r="EZ1" s="69"/>
+      <c r="FA1" s="69"/>
+      <c r="FB1" s="69"/>
+      <c r="FC1" s="69"/>
+      <c r="FD1" s="69"/>
+      <c r="FE1" s="69"/>
     </row>
     <row r="2" spans="1:161">
-      <c r="A2" s="62"/>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="62"/>
-      <c r="AI2" s="62"/>
-      <c r="AJ2" s="62"/>
-      <c r="AK2" s="62"/>
-      <c r="AL2" s="62"/>
-      <c r="AM2" s="62"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="62"/>
-      <c r="AP2" s="62"/>
-      <c r="AQ2" s="62"/>
-      <c r="AR2" s="62"/>
-      <c r="AS2" s="62"/>
-      <c r="AT2" s="62"/>
-      <c r="AU2" s="62"/>
-      <c r="AV2" s="62"/>
-      <c r="AW2" s="62"/>
-      <c r="AX2" s="62"/>
-      <c r="AY2" s="62"/>
-      <c r="AZ2" s="62"/>
-      <c r="BA2" s="62"/>
-      <c r="BB2" s="62"/>
-      <c r="BC2" s="62"/>
-      <c r="BD2" s="62"/>
-      <c r="BE2" s="62"/>
-      <c r="BF2" s="62"/>
-      <c r="BG2" s="62"/>
-      <c r="BH2" s="62"/>
-      <c r="BI2" s="62"/>
-      <c r="BJ2" s="62"/>
-      <c r="BK2" s="62"/>
-      <c r="BL2" s="63"/>
-      <c r="BM2" s="63"/>
-      <c r="BN2" s="63"/>
-      <c r="BO2" s="63"/>
-      <c r="BP2" s="63"/>
-      <c r="BQ2" s="63"/>
-      <c r="BR2" s="63"/>
-      <c r="BS2" s="63"/>
-      <c r="BT2" s="63"/>
-      <c r="BU2" s="63"/>
-      <c r="BV2" s="63"/>
-      <c r="BW2" s="63"/>
-      <c r="BX2" s="63"/>
-      <c r="BY2" s="63"/>
-      <c r="BZ2" s="63"/>
-      <c r="CA2" s="63"/>
-      <c r="CB2" s="63"/>
-      <c r="CC2" s="63"/>
-      <c r="CD2" s="63"/>
-      <c r="CE2" s="63"/>
-      <c r="CF2" s="63"/>
-      <c r="CG2" s="62" t="s">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
+      <c r="W2" s="67"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="67"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
+      <c r="AC2" s="67"/>
+      <c r="AD2" s="67"/>
+      <c r="AE2" s="67"/>
+      <c r="AF2" s="67"/>
+      <c r="AG2" s="67"/>
+      <c r="AH2" s="67"/>
+      <c r="AI2" s="67"/>
+      <c r="AJ2" s="67"/>
+      <c r="AK2" s="67"/>
+      <c r="AL2" s="67"/>
+      <c r="AM2" s="67"/>
+      <c r="AN2" s="67"/>
+      <c r="AO2" s="67"/>
+      <c r="AP2" s="67"/>
+      <c r="AQ2" s="67"/>
+      <c r="AR2" s="67"/>
+      <c r="AS2" s="67"/>
+      <c r="AT2" s="67"/>
+      <c r="AU2" s="67"/>
+      <c r="AV2" s="67"/>
+      <c r="AW2" s="67"/>
+      <c r="AX2" s="67"/>
+      <c r="AY2" s="67"/>
+      <c r="AZ2" s="67"/>
+      <c r="BA2" s="67"/>
+      <c r="BB2" s="67"/>
+      <c r="BC2" s="67"/>
+      <c r="BD2" s="67"/>
+      <c r="BE2" s="67"/>
+      <c r="BF2" s="67"/>
+      <c r="BG2" s="67"/>
+      <c r="BH2" s="67"/>
+      <c r="BI2" s="67"/>
+      <c r="BJ2" s="67"/>
+      <c r="BK2" s="67"/>
+      <c r="BL2" s="68"/>
+      <c r="BM2" s="68"/>
+      <c r="BN2" s="68"/>
+      <c r="BO2" s="68"/>
+      <c r="BP2" s="68"/>
+      <c r="BQ2" s="68"/>
+      <c r="BR2" s="68"/>
+      <c r="BS2" s="68"/>
+      <c r="BT2" s="68"/>
+      <c r="BU2" s="68"/>
+      <c r="BV2" s="68"/>
+      <c r="BW2" s="68"/>
+      <c r="BX2" s="68"/>
+      <c r="BY2" s="68"/>
+      <c r="BZ2" s="68"/>
+      <c r="CA2" s="68"/>
+      <c r="CB2" s="68"/>
+      <c r="CC2" s="68"/>
+      <c r="CD2" s="68"/>
+      <c r="CE2" s="68"/>
+      <c r="CF2" s="68"/>
+      <c r="CG2" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="CH2" s="62"/>
-      <c r="CI2" s="62"/>
-      <c r="CJ2" s="62"/>
-      <c r="CK2" s="62"/>
-      <c r="CL2" s="62"/>
-      <c r="CM2" s="62"/>
-      <c r="CN2" s="62" t="s">
+      <c r="CH2" s="67"/>
+      <c r="CI2" s="67"/>
+      <c r="CJ2" s="67"/>
+      <c r="CK2" s="67"/>
+      <c r="CL2" s="67"/>
+      <c r="CM2" s="67"/>
+      <c r="CN2" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="CO2" s="62"/>
-      <c r="CP2" s="62"/>
-      <c r="CQ2" s="62"/>
-      <c r="CR2" s="62"/>
-      <c r="CS2" s="62"/>
-      <c r="CT2" s="62"/>
-      <c r="CU2" s="62" t="s">
+      <c r="CO2" s="67"/>
+      <c r="CP2" s="67"/>
+      <c r="CQ2" s="67"/>
+      <c r="CR2" s="67"/>
+      <c r="CS2" s="67"/>
+      <c r="CT2" s="67"/>
+      <c r="CU2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="CV2" s="62"/>
-      <c r="CW2" s="62"/>
-      <c r="CX2" s="62"/>
-      <c r="CY2" s="62"/>
-      <c r="CZ2" s="62"/>
-      <c r="DA2" s="62"/>
-      <c r="DB2" s="62" t="s">
+      <c r="CV2" s="67"/>
+      <c r="CW2" s="67"/>
+      <c r="CX2" s="67"/>
+      <c r="CY2" s="67"/>
+      <c r="CZ2" s="67"/>
+      <c r="DA2" s="67"/>
+      <c r="DB2" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="DC2" s="62"/>
-      <c r="DD2" s="62"/>
-      <c r="DE2" s="62"/>
-      <c r="DF2" s="62"/>
-      <c r="DG2" s="62"/>
-      <c r="DH2" s="62"/>
-      <c r="DI2" s="62" t="s">
+      <c r="DC2" s="67"/>
+      <c r="DD2" s="67"/>
+      <c r="DE2" s="67"/>
+      <c r="DF2" s="67"/>
+      <c r="DG2" s="67"/>
+      <c r="DH2" s="67"/>
+      <c r="DI2" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="DJ2" s="62"/>
-      <c r="DK2" s="62"/>
-      <c r="DL2" s="62"/>
-      <c r="DM2" s="62"/>
-      <c r="DN2" s="62"/>
-      <c r="DO2" s="62"/>
-      <c r="DP2" s="62" t="s">
+      <c r="DJ2" s="67"/>
+      <c r="DK2" s="67"/>
+      <c r="DL2" s="67"/>
+      <c r="DM2" s="67"/>
+      <c r="DN2" s="67"/>
+      <c r="DO2" s="67"/>
+      <c r="DP2" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="DQ2" s="62"/>
-      <c r="DR2" s="62"/>
-      <c r="DS2" s="62"/>
-      <c r="DT2" s="62"/>
-      <c r="DU2" s="62"/>
-      <c r="DV2" s="62"/>
-      <c r="DW2" s="62" t="s">
+      <c r="DQ2" s="67"/>
+      <c r="DR2" s="67"/>
+      <c r="DS2" s="67"/>
+      <c r="DT2" s="67"/>
+      <c r="DU2" s="67"/>
+      <c r="DV2" s="67"/>
+      <c r="DW2" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="DX2" s="62"/>
-      <c r="DY2" s="62"/>
-      <c r="DZ2" s="62"/>
-      <c r="EA2" s="62"/>
-      <c r="EB2" s="62"/>
-      <c r="EC2" s="62"/>
-      <c r="ED2" s="62"/>
-      <c r="EE2" s="62"/>
-      <c r="EF2" s="62"/>
-      <c r="EG2" s="62"/>
-      <c r="EH2" s="62"/>
-      <c r="EI2" s="62"/>
-      <c r="EJ2" s="62"/>
-      <c r="EK2" s="61" t="s">
+      <c r="DX2" s="67"/>
+      <c r="DY2" s="67"/>
+      <c r="DZ2" s="67"/>
+      <c r="EA2" s="67"/>
+      <c r="EB2" s="67"/>
+      <c r="EC2" s="67"/>
+      <c r="ED2" s="67"/>
+      <c r="EE2" s="67"/>
+      <c r="EF2" s="67"/>
+      <c r="EG2" s="67"/>
+      <c r="EH2" s="67"/>
+      <c r="EI2" s="67"/>
+      <c r="EJ2" s="67"/>
+      <c r="EK2" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="EL2" s="61"/>
-      <c r="EM2" s="61"/>
-      <c r="EN2" s="61"/>
-      <c r="EO2" s="61"/>
-      <c r="EP2" s="61"/>
-      <c r="EQ2" s="61"/>
-      <c r="ER2" s="61" t="s">
+      <c r="EL2" s="69"/>
+      <c r="EM2" s="69"/>
+      <c r="EN2" s="69"/>
+      <c r="EO2" s="69"/>
+      <c r="EP2" s="69"/>
+      <c r="EQ2" s="69"/>
+      <c r="ER2" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="ES2" s="61"/>
-      <c r="ET2" s="61"/>
-      <c r="EU2" s="61"/>
-      <c r="EV2" s="61"/>
-      <c r="EW2" s="61"/>
-      <c r="EX2" s="61"/>
-      <c r="EY2" s="61" t="s">
+      <c r="ES2" s="69"/>
+      <c r="ET2" s="69"/>
+      <c r="EU2" s="69"/>
+      <c r="EV2" s="69"/>
+      <c r="EW2" s="69"/>
+      <c r="EX2" s="69"/>
+      <c r="EY2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="EZ2" s="61"/>
-      <c r="FA2" s="61"/>
-      <c r="FB2" s="61"/>
-      <c r="FC2" s="61"/>
-      <c r="FD2" s="61"/>
-      <c r="FE2" s="61"/>
+      <c r="EZ2" s="69"/>
+      <c r="FA2" s="69"/>
+      <c r="FB2" s="69"/>
+      <c r="FC2" s="69"/>
+      <c r="FD2" s="69"/>
+      <c r="FE2" s="69"/>
     </row>
     <row r="3" spans="1:161">
       <c r="E3" s="1">
@@ -3430,27 +3435,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="BL1:BR2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:J2"/>
-    <mergeCell ref="K1:R2"/>
-    <mergeCell ref="S1:AA2"/>
-    <mergeCell ref="AB1:AI2"/>
-    <mergeCell ref="AJ1:AP2"/>
-    <mergeCell ref="AQ1:AW2"/>
-    <mergeCell ref="AX1:BD2"/>
-    <mergeCell ref="BE1:BK2"/>
-    <mergeCell ref="EK1:EQ1"/>
-    <mergeCell ref="ER1:EX1"/>
-    <mergeCell ref="BS1:BY2"/>
-    <mergeCell ref="BZ1:CF2"/>
-    <mergeCell ref="CG1:CM1"/>
-    <mergeCell ref="CN1:CT1"/>
-    <mergeCell ref="CU1:DA1"/>
-    <mergeCell ref="DB1:DH1"/>
-    <mergeCell ref="ER2:EX2"/>
     <mergeCell ref="EY2:FE2"/>
     <mergeCell ref="EY1:FE1"/>
     <mergeCell ref="CG2:CM2"/>
@@ -3466,6 +3450,27 @@
     <mergeCell ref="DP1:DV1"/>
     <mergeCell ref="DW1:EC1"/>
     <mergeCell ref="ED1:EJ1"/>
+    <mergeCell ref="EK1:EQ1"/>
+    <mergeCell ref="ER1:EX1"/>
+    <mergeCell ref="BS1:BY2"/>
+    <mergeCell ref="BZ1:CF2"/>
+    <mergeCell ref="CG1:CM1"/>
+    <mergeCell ref="CN1:CT1"/>
+    <mergeCell ref="CU1:DA1"/>
+    <mergeCell ref="DB1:DH1"/>
+    <mergeCell ref="ER2:EX2"/>
+    <mergeCell ref="BL1:BR2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:J2"/>
+    <mergeCell ref="K1:R2"/>
+    <mergeCell ref="S1:AA2"/>
+    <mergeCell ref="AB1:AI2"/>
+    <mergeCell ref="AJ1:AP2"/>
+    <mergeCell ref="AQ1:AW2"/>
+    <mergeCell ref="AX1:BD2"/>
+    <mergeCell ref="BE1:BK2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3475,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C670FF-1803-F745-A230-8EE7EF83CC20}">
   <dimension ref="A3:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3491,22 +3496,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
       <c r="J4" t="s">
         <v>83</v>
       </c>
@@ -3515,11 +3520,11 @@
       <c r="A5" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="70"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="76"/>
       <c r="J5" t="s">
         <v>84</v>
       </c>
@@ -3528,11 +3533,11 @@
       <c r="A6" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
       <c r="J6" t="s">
         <v>85</v>
       </c>
@@ -3541,10 +3546,10 @@
       <c r="A7" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="74">
+      <c r="B7" s="63">
         <v>35551</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="64" t="s">
         <v>130</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -3555,11 +3560,11 @@
       <c r="A8" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="67">
+      <c r="B8" s="73">
         <v>34.15</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="J8" t="s">
         <v>88</v>
       </c>
@@ -3568,21 +3573,21 @@
       <c r="A9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="68">
+      <c r="B9" s="74">
         <v>819</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="70"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="68">
+      <c r="B10" s="74">
         <v>28</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="70"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
       <c r="E10" s="42" t="s">
         <v>97</v>
       </c>
@@ -3594,17 +3599,17 @@
       <c r="A11" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="67">
+      <c r="B11" s="73">
         <v>4810</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="71" t="s">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77"/>
       <c r="J11" t="s">
         <v>86</v>
       </c>
@@ -3613,26 +3618,26 @@
       <c r="A12" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
       <c r="J12" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
+      <c r="A14" s="61"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="18" t="s">
@@ -3647,7 +3652,7 @@
       <c r="D16" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="77"/>
+      <c r="E16" s="66"/>
       <c r="J16" t="s">
         <v>90</v>
       </c>
@@ -3666,7 +3671,7 @@
         <f>(C17-B17)/B17</f>
         <v>-0.14901787032934574</v>
       </c>
-      <c r="E17" s="76"/>
+      <c r="E17" s="65"/>
       <c r="J17" t="s">
         <v>91</v>
       </c>
@@ -3685,7 +3690,7 @@
         <f>(C18-B18)/B18</f>
         <v>-0.11805246776345042</v>
       </c>
-      <c r="E18" s="76"/>
+      <c r="E18" s="65"/>
       <c r="J18" t="s">
         <v>92</v>
       </c>
@@ -3704,7 +3709,7 @@
         <f>(C19-B19)/B19</f>
         <v>-0.16439992038744775</v>
       </c>
-      <c r="E19" s="76"/>
+      <c r="E19" s="65"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31" t="s">
@@ -3713,7 +3718,7 @@
       <c r="B20" s="24"/>
       <c r="C20" s="24"/>
       <c r="D20" s="21"/>
-      <c r="E20" s="76"/>
+      <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31" t="s">
@@ -3722,24 +3727,24 @@
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
-      <c r="E21" s="76"/>
+      <c r="E21" s="65"/>
       <c r="J21" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="72"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="72"/>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
     </row>
     <row r="24" spans="1:10">
       <c r="J24" t="s">
@@ -4060,7 +4065,7 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="F37" s="64" t="s">
+      <c r="F37" s="70" t="s">
         <v>126</v>
       </c>
       <c r="G37" s="59" t="s">
@@ -4068,7 +4073,7 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="F38" s="64"/>
+      <c r="F38" s="70"/>
       <c r="G38" s="60" t="s">
         <v>128</v>
       </c>
@@ -4207,28 +4212,28 @@
       <c r="E49" s="27"/>
     </row>
     <row r="52" spans="1:9">
-      <c r="B52" s="62">
-        <v>2017</v>
-      </c>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62">
-        <v>2018</v>
-      </c>
-      <c r="G52" s="62"/>
-      <c r="H52" s="62"/>
-      <c r="I52" s="62"/>
+      <c r="B52" s="67">
+        <v>2017</v>
+      </c>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67">
+        <v>2018</v>
+      </c>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="67"/>
     </row>
     <row r="53" spans="1:9">
-      <c r="B53" s="62" t="s">
+      <c r="B53" s="67" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62" t="s">
+      <c r="C53" s="67"/>
+      <c r="D53" s="67" t="s">
         <v>122</v>
       </c>
-      <c r="E53" s="62"/>
+      <c r="E53" s="67"/>
       <c r="F53" s="2" t="s">
         <v>121</v>
       </c>
@@ -4440,54 +4445,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="67"/>
+      <c r="R1" s="67"/>
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
     </row>
     <row r="2" spans="2:22">
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="62"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="67"/>
     </row>
     <row r="3" spans="2:22">
       <c r="B3">

</xml_diff>